<commit_message>
update district level data
</commit_message>
<xml_diff>
--- a/data-raw/Malaria Readiness Assessment_District.xlsx
+++ b/data-raw/Malaria Readiness Assessment_District.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Robinson/Afenet-projects/afenet-uganda/malariaRA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2CAB45-2524-5847-9C04-144C8B8A107F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949608BB-6117-5542-9EA5-ADEC9E7BCEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -872,9 +872,6 @@
     <t>health_workers_trained_2.1</t>
   </si>
   <si>
-    <t>Com_health_volunteers_trained_2.2</t>
-  </si>
-  <si>
     <t>supervisors_identified_and_trained_2.3</t>
   </si>
   <si>
@@ -893,15 +890,6 @@
     <t>waste_mgt_assessment_4.2</t>
   </si>
   <si>
-    <t>vaccines_4.4a</t>
-  </si>
-  <si>
-    <t>safety_boxes_4.4d</t>
-  </si>
-  <si>
-    <t>additional_commodities_4.4e</t>
-  </si>
-  <si>
     <t>acsm_mgt_delivered_5.1</t>
   </si>
   <si>
@@ -983,27 +971,6 @@
     <t>1wk</t>
   </si>
   <si>
-    <t xml:space="preserve">4.4b 0.5ml AD syringes </t>
-  </si>
-  <si>
-    <t>4.4a Vaccines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.4c 2ml RUP reconstitution syringes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.4d Safety boxes </t>
-  </si>
-  <si>
-    <t>4.4e (If relevant) additional commodities (such as vitamin A, deworming, insecticide-treated bed nets etc.)</t>
-  </si>
-  <si>
-    <t>AD_syringes_0.5ml_4.4b</t>
-  </si>
-  <si>
-    <t>RUP_reconstitution_syringes_2ml_4.4c</t>
-  </si>
-  <si>
     <t>malaria_readiness_assessment</t>
   </si>
   <si>
@@ -1011,6 +978,39 @@
   </si>
   <si>
     <t>1 Month</t>
+  </si>
+  <si>
+    <t>1.6 Monthly coordination meeting at district level led by the district task force chaired by the RDC</t>
+  </si>
+  <si>
+    <t>funds_distributed_1_6</t>
+  </si>
+  <si>
+    <t>com_health_volunteers_trained_2_2</t>
+  </si>
+  <si>
+    <t>vaccines_mgt_supplied_vaccines_4_3a</t>
+  </si>
+  <si>
+    <t>vaccines_mgt_supplied_ad_syringes_0_5ml_4_3b</t>
+  </si>
+  <si>
+    <t>vaccines_mgt_supplied_safety_boxes_4_3c</t>
+  </si>
+  <si>
+    <t>vaccines_mgt_supplied_comments_cold_chain_and_logistics</t>
+  </si>
+  <si>
+    <t>4.3a Vaccines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.3b 0.5ml AD syringes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.3c Safety boxes </t>
+  </si>
+  <si>
+    <t>4.3e (If relevant) additional commodities (such as vitamin A, deworming, insecticide-treated bed nets etc.)</t>
   </si>
 </sst>
 </file>
@@ -1577,15 +1577,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M223"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
     <col min="3" max="3" width="83.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -1928,7 +1928,7 @@
         <v>266</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1942,7 +1942,7 @@
         <v>267</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -1956,7 +1956,7 @@
         <v>268</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1970,7 +1970,7 @@
         <v>269</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -1984,35 +1984,35 @@
         <v>270</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -2020,10 +2020,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -2034,38 +2034,38 @@
         <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>273</v>
+        <v>310</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B33" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E33" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2073,10 +2073,10 @@
         <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E34" t="s">
         <v>16</v>
@@ -2087,38 +2087,38 @@
         <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B37" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C37" s="14" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C37" t="s">
-        <v>297</v>
-      </c>
-      <c r="E37" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2126,41 +2126,41 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C38" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E38" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" t="s">
+        <v>294</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B40" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C39" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="L39" t="s">
+      <c r="C40" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="L40" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C40" t="s">
-        <v>310</v>
-      </c>
-      <c r="E40" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2168,10 +2168,10 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C41" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="E41" t="s">
         <v>16</v>
@@ -2182,10 +2182,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C42" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E42" t="s">
         <v>16</v>
@@ -2196,10 +2196,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E43" t="s">
         <v>16</v>
@@ -2210,10 +2210,10 @@
         <v>36</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="C44" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="E44" t="s">
         <v>16</v>
@@ -2243,10 +2243,10 @@
         <v>36</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C47" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E47" t="s">
         <v>16</v>
@@ -2257,10 +2257,10 @@
         <v>36</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C48" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E48" t="s">
         <v>16</v>
@@ -2271,10 +2271,10 @@
         <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E49" t="s">
         <v>16</v>
@@ -2285,10 +2285,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>85</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3334,8 +3334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -3521,7 +3521,7 @@
         <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C20" t="s">
         <v>81</v>
@@ -3532,7 +3532,7 @@
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C21" t="s">
         <v>82</v>
@@ -3543,10 +3543,10 @@
         <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C22" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3554,7 +3554,7 @@
         <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C23" t="s">
         <v>83</v>
@@ -3565,7 +3565,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C24" t="s">
         <v>84</v>
@@ -6290,7 +6290,7 @@
         <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>

</xml_diff>